<commit_message>
Compiler working, I think :)
</commit_message>
<xml_diff>
--- a/documents/Vocabulary.xlsx
+++ b/documents/Vocabulary.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PaulRobson\Projects\flat\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{79B9D01D-B533-4FBB-B4F6-DB3D24DB76DF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FFF854-A87F-40AC-A29D-86F6EA66FC32}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="109">
   <si>
     <t>Word</t>
   </si>
@@ -49,9 +49,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>A = B - A</t>
-  </si>
-  <si>
     <t>!</t>
   </si>
   <si>
@@ -79,12 +76,6 @@
     <t>Compile word in A into memory</t>
   </si>
   <si>
-    <t>/</t>
-  </si>
-  <si>
-    <t>A = B / A</t>
-  </si>
-  <si>
     <t>;</t>
   </si>
   <si>
@@ -127,12 +118,6 @@
     <t>Set A to -1 if A == B, otherwise A = 0</t>
   </si>
   <si>
-    <t>0-</t>
-  </si>
-  <si>
-    <t>Negate A</t>
-  </si>
-  <si>
     <t>0&lt;</t>
   </si>
   <si>
@@ -280,12 +265,6 @@
     <t>A-&gt;B, A becomes key press</t>
   </si>
   <si>
-    <t>mod</t>
-  </si>
-  <si>
-    <t>A = B mod A</t>
-  </si>
-  <si>
     <t>module</t>
   </si>
   <si>
@@ -365,12 +344,15 @@
   </si>
   <si>
     <t>A = A xor B</t>
+  </si>
+  <si>
+    <t>A = -A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -636,41 +618,41 @@
     </xf>
   </cellXfs>
   <cellStyles count="35">
-    <cellStyle name="Accent" xfId="7"/>
-    <cellStyle name="Accent 1" xfId="8"/>
-    <cellStyle name="Accent 1 5" xfId="9"/>
-    <cellStyle name="Accent 2" xfId="10"/>
-    <cellStyle name="Accent 2 6" xfId="11"/>
-    <cellStyle name="Accent 3" xfId="12"/>
-    <cellStyle name="Accent 3 7" xfId="13"/>
-    <cellStyle name="Accent 4" xfId="14"/>
+    <cellStyle name="Accent" xfId="7" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Accent 1" xfId="8" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Accent 1 5" xfId="9" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Accent 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Accent 2 6" xfId="11" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Accent 3" xfId="12" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Accent 3 7" xfId="13" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Accent 4" xfId="14" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Bad" xfId="4" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Error" xfId="15"/>
-    <cellStyle name="Error 8" xfId="16"/>
-    <cellStyle name="Excel Built-in Bad" xfId="17"/>
-    <cellStyle name="Excel Built-in Good" xfId="18"/>
-    <cellStyle name="Excel Built-in Heading 1" xfId="19"/>
-    <cellStyle name="Excel Built-in Heading 2" xfId="20"/>
-    <cellStyle name="Excel Built-in Neutral" xfId="21"/>
-    <cellStyle name="Excel Built-in Note" xfId="22"/>
-    <cellStyle name="Footnote" xfId="23"/>
-    <cellStyle name="Footnote 9" xfId="24"/>
+    <cellStyle name="Error" xfId="15" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Error 8" xfId="16" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Excel Built-in Bad" xfId="17" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Excel Built-in Good" xfId="18" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Excel Built-in Heading 1" xfId="19" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Excel Built-in Heading 2" xfId="20" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Excel Built-in Neutral" xfId="21" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Excel Built-in Note" xfId="22" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Footnote" xfId="23" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Footnote 9" xfId="24" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
     <cellStyle name="Good" xfId="3" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading" xfId="25"/>
+    <cellStyle name="Heading" xfId="25" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 10" xfId="26"/>
+    <cellStyle name="Heading 10" xfId="26" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="27"/>
-    <cellStyle name="Hyperlink 11" xfId="28"/>
+    <cellStyle name="Hyperlink" xfId="27" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Hyperlink 11" xfId="28" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
     <cellStyle name="Neutral" xfId="5" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Note" xfId="6" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Status" xfId="29"/>
-    <cellStyle name="Status 12" xfId="30"/>
-    <cellStyle name="Text" xfId="31"/>
-    <cellStyle name="Text 13" xfId="32"/>
-    <cellStyle name="Warning" xfId="33"/>
-    <cellStyle name="Warning 14" xfId="34"/>
+    <cellStyle name="Status" xfId="29" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Status 12" xfId="30" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Text" xfId="31" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Text 13" xfId="32" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Warning" xfId="33" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Warning 14" xfId="34" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -981,10 +963,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1036,194 +1020,194 @@
         <v>6</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>9</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="6" t="s">
+    </row>
+    <row r="8" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="B8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
     </row>
     <row r="9" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
     </row>
     <row r="10" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
     </row>
     <row r="11" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
     </row>
     <row r="12" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
     </row>
     <row r="13" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>30</v>
       </c>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
     </row>
     <row r="14" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
     </row>
     <row r="15" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
     </row>
     <row r="16" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>5</v>
@@ -1232,14 +1216,14 @@
         <v>6</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
     </row>
     <row r="17" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>5</v>
@@ -1248,14 +1232,14 @@
         <v>6</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
     </row>
     <row r="18" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>5</v>
@@ -1266,511 +1250,465 @@
       <c r="D18" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
     </row>
     <row r="19" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
     </row>
     <row r="20" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>56</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>58</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="6" t="s">
         <v>72</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="6" t="s">
         <v>74</v>
-      </c>
-      <c r="B36" s="3"/>
-      <c r="C36" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D39" s="6" t="s">
+    </row>
+    <row r="40" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="5" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="6" t="s">
         <v>84</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" s="6" t="s">
+    </row>
+    <row r="43" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
+      <c r="B43" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="6" t="s">
         <v>88</v>
-      </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="6" t="s">
         <v>90</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="6" t="s">
         <v>92</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="6" t="s">
         <v>94</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B48" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" s="6" t="s">
+    </row>
+    <row r="49" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
+      <c r="B49" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" s="6" t="s">
         <v>100</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" s="6" t="s">
         <v>102</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B51" s="3"/>
+      <c r="C51" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B51" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D51" s="6" t="s">
+    </row>
+    <row r="52" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
+      <c r="B52" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" s="5" t="s">
         <v>106</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>6</v>
       </c>
       <c r="D52" s="6" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="B54" s="3"/>
-      <c r="C54" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D55" s="6" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started work on command line
</commit_message>
<xml_diff>
--- a/documents/Vocabulary.xlsx
+++ b/documents/Vocabulary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PaulRobson\Projects\flat\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FFF854-A87F-40AC-A29D-86F6EA66FC32}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD4C697-E5E8-4B3C-9940-78343ECA2FB5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="110">
   <si>
     <t>Word</t>
   </si>
@@ -347,6 +347,9 @@
   </si>
   <si>
     <t>A = -A</t>
+  </si>
+  <si>
+    <t>Tested</t>
   </si>
 </sst>
 </file>
@@ -966,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1000,7 +1003,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>6</v>
@@ -1014,7 +1017,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>6</v>
@@ -1028,7 +1031,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>6</v>
@@ -1053,8 +1056,8 @@
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>5</v>
+      <c r="B6" s="4" t="s">
+        <v>109</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>6</v>
@@ -1067,8 +1070,8 @@
       <c r="A7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>5</v>
+      <c r="B7" s="4" t="s">
+        <v>109</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>6</v>
@@ -1082,7 +1085,7 @@
         <v>18</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>6</v>
@@ -1098,7 +1101,7 @@
         <v>20</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>6</v>
@@ -1114,7 +1117,7 @@
         <v>22</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>6</v>
@@ -1130,7 +1133,7 @@
         <v>24</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>6</v>
@@ -1146,7 +1149,7 @@
         <v>26</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>6</v>
@@ -1162,7 +1165,7 @@
         <v>28</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>6</v>
@@ -1177,8 +1180,8 @@
       <c r="A14" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>5</v>
+      <c r="B14" s="4" t="s">
+        <v>109</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>6</v>
@@ -1194,7 +1197,7 @@
         <v>32</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>6</v>
@@ -1210,7 +1213,7 @@
         <v>34</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>6</v>
@@ -1226,7 +1229,7 @@
         <v>35</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>6</v>
@@ -1242,7 +1245,7 @@
         <v>37</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>6</v>
@@ -1256,7 +1259,7 @@
         <v>39</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>6</v>
@@ -1270,7 +1273,7 @@
         <v>41</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>6</v>
@@ -1284,7 +1287,7 @@
         <v>43</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>6</v>
@@ -1321,8 +1324,8 @@
       <c r="A24" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>5</v>
+      <c r="B24" s="4" t="s">
+        <v>109</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>6</v>
@@ -1335,8 +1338,8 @@
       <c r="A25" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>5</v>
+      <c r="B25" s="4" t="s">
+        <v>109</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>6</v>
@@ -1350,7 +1353,7 @@
         <v>53</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>6</v>
@@ -1363,8 +1366,8 @@
       <c r="A27" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>5</v>
+      <c r="B27" s="4" t="s">
+        <v>109</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>6</v>
@@ -1378,7 +1381,7 @@
         <v>57</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>6</v>
@@ -1391,8 +1394,8 @@
       <c r="A29" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>5</v>
+      <c r="B29" s="4" t="s">
+        <v>109</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>6</v>
@@ -1445,8 +1448,8 @@
       <c r="A33" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>5</v>
+      <c r="B33" s="4" t="s">
+        <v>109</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>6</v>
@@ -1471,8 +1474,8 @@
       <c r="A35" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>5</v>
+      <c r="B35" s="4" t="s">
+        <v>109</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>6</v>
@@ -1486,7 +1489,7 @@
         <v>73</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>6</v>
@@ -1523,8 +1526,8 @@
       <c r="A39" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>5</v>
+      <c r="B39" s="4" t="s">
+        <v>109</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>6</v>
@@ -1550,7 +1553,7 @@
         <v>83</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>6</v>
@@ -1564,7 +1567,7 @@
         <v>85</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>6</v>
@@ -1578,7 +1581,7 @@
         <v>87</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>6</v>
@@ -1592,7 +1595,7 @@
         <v>89</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>6</v>
@@ -1606,7 +1609,7 @@
         <v>91</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>6</v>
@@ -1620,7 +1623,7 @@
         <v>93</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>6</v>
@@ -1634,7 +1637,7 @@
         <v>95</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>6</v>
@@ -1648,7 +1651,7 @@
         <v>97</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>6</v>
@@ -1661,8 +1664,8 @@
       <c r="A49" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B49" s="3" t="s">
-        <v>5</v>
+      <c r="B49" s="4" t="s">
+        <v>109</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>6</v>
@@ -1676,7 +1679,7 @@
         <v>101</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>6</v>
@@ -1702,7 +1705,7 @@
         <v>105</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>106</v>

</xml_diff>